<commit_message>
what we need to do
</commit_message>
<xml_diff>
--- a/Codebook Uganda Panel.xlsx
+++ b/Codebook Uganda Panel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/Master thesis/MLhetrogeneouseffects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B08050-94DB-8D48-A8CE-9F97CA4478B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78A343A-A46B-A542-B61E-B07D19CAE58E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="500" windowWidth="28040" windowHeight="16540" xr2:uid="{4A1EAC35-01F1-A54B-8647-BEC3205DBE2C}"/>
+    <workbookView xWindow="3320" yWindow="500" windowWidth="28040" windowHeight="16540" activeTab="1" xr2:uid="{4A1EAC35-01F1-A54B-8647-BEC3205DBE2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="325">
   <si>
     <t>Attitude</t>
   </si>
@@ -754,13 +755,259 @@
   </si>
   <si>
     <t>No=0, yes=1 (if never worry she will get a job)</t>
+  </si>
+  <si>
+    <t>Otherwise=0, yes=1</t>
+  </si>
+  <si>
+    <t>No=0, yes=1 (at least maybe)</t>
+  </si>
+  <si>
+    <t>from 0 to 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HIV knowledge index is based on the number of statements correctly identified as true or false. Therelevant statements are "A person who has HIV is different from a person who is ill with AIDS", "During vaginal sex, it is easier for a woman to receivethe HIV virus than for a man", "Pulling out the penis before a man climaxes keeps a women from getting HIV during sex", "A women cannot get HIV ifshe has sex during her period", "Taking a test for HIV one week after having sex will tell a person if she or he has HIV." and "A Pregnant woman withHIV can give the virus to her unborn baby". </t>
+  </si>
+  <si>
+    <t>The pregnancy knowledge index equals 1 if the respondent correctly identifies the statement "A womencannot become pregnant at first intercourse or with occasional sexual relations" as true or false.</t>
+  </si>
+  <si>
+    <t>The index for satisfaction withearnings/income is the reveresed and rescaled respondent's self-assessment on a 7 point score (where originally "1" is completely happy and "7" is notat all happy) The top 1% outliers of the expenditure variable have been removed.</t>
+  </si>
+  <si>
+    <t>0=not satisfied, 6=completely happy</t>
+  </si>
+  <si>
+    <t>Follow up</t>
+  </si>
+  <si>
+    <t>Endline</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Need to standardize</t>
+  </si>
+  <si>
+    <t>Rename to a dummy</t>
+  </si>
+  <si>
+    <t>z_empowerment</t>
+  </si>
+  <si>
+    <t>hsworked_year_empl</t>
+  </si>
+  <si>
+    <t>hsworked_self_empl</t>
+  </si>
+  <si>
+    <t>Qhsworked_year_empl</t>
+  </si>
+  <si>
+    <t>Qhsworked_self_empl</t>
+  </si>
+  <si>
+    <t>Rhsworked_self_empl</t>
+  </si>
+  <si>
+    <t>Rhsworked_year_empl</t>
+  </si>
+  <si>
+    <t>Trimmed variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Description: this chart only contain variables according to the columns labels. Other variables that are included in the sample but do not fit in the columns categories are not included here. </t>
+  </si>
+  <si>
+    <t>incind_self_empl</t>
+  </si>
+  <si>
+    <t>income_year_int</t>
+  </si>
+  <si>
+    <t>lifeskillsMOREfew</t>
+  </si>
+  <si>
+    <t>Too many missings more than 50% = delete</t>
+  </si>
+  <si>
+    <t>livelihoodMOREfew</t>
+  </si>
+  <si>
+    <t>other_contraceptive</t>
+  </si>
+  <si>
+    <t>satisfaction_income</t>
+  </si>
+  <si>
+    <t>self_empl</t>
+  </si>
+  <si>
+    <t>age_Imarry</t>
+  </si>
+  <si>
+    <t>Rage_Imarry</t>
+  </si>
+  <si>
+    <t>age_imarry --&gt; can teach us if expectation about marriage change following the intervention probably women would want to marry later</t>
+  </si>
+  <si>
+    <t>RM_marrywhox</t>
+  </si>
+  <si>
+    <t>M_marrywhox</t>
+  </si>
+  <si>
+    <t>rural</t>
+  </si>
+  <si>
+    <t>rich</t>
+  </si>
+  <si>
+    <t>below16</t>
+  </si>
+  <si>
+    <t>QM_chi</t>
+  </si>
+  <si>
+    <t>Variables we can delete</t>
+  </si>
+  <si>
+    <t>Q_part</t>
+  </si>
+  <si>
+    <t>QR_sexu</t>
+  </si>
+  <si>
+    <t>Qsex_p</t>
+  </si>
+  <si>
+    <t>Qrhiv_s</t>
+  </si>
+  <si>
+    <t>Qalways_c</t>
+  </si>
+  <si>
+    <t>Qother_c</t>
+  </si>
+  <si>
+    <t>QM_i_ageF</t>
+  </si>
+  <si>
+    <t>QM_i_ageM</t>
+  </si>
+  <si>
+    <t>QM_baby_ageF</t>
+  </si>
+  <si>
+    <t>QM_daught</t>
+  </si>
+  <si>
+    <t>QM_son</t>
+  </si>
+  <si>
+    <t>Qaspiration</t>
+  </si>
+  <si>
+    <t>Qiga (we are not sure what this variable is)</t>
+  </si>
+  <si>
+    <t>RM_chi</t>
+  </si>
+  <si>
+    <t>Rpart</t>
+  </si>
+  <si>
+    <t>RR_sexu</t>
+  </si>
+  <si>
+    <t>Rsex_p</t>
+  </si>
+  <si>
+    <t>RRhiv_s</t>
+  </si>
+  <si>
+    <t>R_always_c</t>
+  </si>
+  <si>
+    <t>Rother_c</t>
+  </si>
+  <si>
+    <t>RM_i_ageF</t>
+  </si>
+  <si>
+    <t>RM_i_ageM</t>
+  </si>
+  <si>
+    <t>RM_baby_ageF</t>
+  </si>
+  <si>
+    <t>RM_baby_ageM</t>
+  </si>
+  <si>
+    <t>RM_daught</t>
+  </si>
+  <si>
+    <t>RM_son</t>
+  </si>
+  <si>
+    <t>Already standardized/index</t>
+  </si>
+  <si>
+    <t>aspiration</t>
+  </si>
+  <si>
+    <t>Raspiration</t>
+  </si>
+  <si>
+    <t>Riga</t>
+  </si>
+  <si>
+    <t>M_chi</t>
+  </si>
+  <si>
+    <t>part (partner reversed)</t>
+  </si>
+  <si>
+    <t>R_sexu</t>
+  </si>
+  <si>
+    <t>sex_p</t>
+  </si>
+  <si>
+    <t>Rhiv_s</t>
+  </si>
+  <si>
+    <t>always_c</t>
+  </si>
+  <si>
+    <t>other_c</t>
+  </si>
+  <si>
+    <t>M_i_ageF</t>
+  </si>
+  <si>
+    <t>M_i_ageM</t>
+  </si>
+  <si>
+    <t>M_baby_no</t>
+  </si>
+  <si>
+    <t>M_baby_ageF</t>
+  </si>
+  <si>
+    <t>M_daught</t>
+  </si>
+  <si>
+    <t>M_son</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -783,16 +1030,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -800,14 +1072,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1122,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D2D18B-3C43-AA4B-B0B6-CA1FC37A728E}">
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,1293 +1469,2269 @@
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="75.33203125" customWidth="1"/>
     <col min="3" max="3" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B12" s="3" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C12" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C14" s="3" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C15" s="3" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B16" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B17" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B18" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B19" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B21" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B22" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C28" s="3" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B29" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C29" s="3" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C30" s="3" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B31" s="3" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B32" s="3" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B33" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C33" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B34" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B35" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B36" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B37" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C37" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C38" s="3" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B39" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C39" s="3" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E63" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E65" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B68" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="C68" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B69" s="6" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C69" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B70" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C70" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B71" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C71" s="6" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="E71" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B72" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="C72" s="6"/>
+      <c r="E72" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B73" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="C73" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B74" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="C74" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B75" s="6" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="C75" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B76" s="6" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="C76" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B77" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="C77" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B78" s="6" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="C78" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B79" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="C79" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B80" s="6" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="C80" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B81" s="6" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="C81" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B82" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="C82" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B83" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="C83" s="6"/>
+      <c r="E83" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B84" s="6" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="C84" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B85" s="6" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="C85" s="6"/>
+      <c r="E85" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B86" s="6" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="C86" s="6"/>
+      <c r="E86" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B87" s="6" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="C87" s="6"/>
+      <c r="E87" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B88" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="C88" s="6"/>
+      <c r="E88" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B89" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="C89" s="6"/>
+      <c r="E89" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B90" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="C90" s="6"/>
+      <c r="E90" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B91" s="6" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="C91" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B92" s="6" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="C92" s="6"/>
+      <c r="E92" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B93" s="6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="C93" s="6"/>
+      <c r="E93" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B94" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C94" s="6" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="E94" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B95" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C95" s="6" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="E95" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B96" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C96" s="6" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="E96" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B97" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C97" s="6" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="E97" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B98" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="C98" s="6"/>
+      <c r="E98" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B99" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="C99" s="6"/>
+      <c r="E99" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B100" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="C100" s="6"/>
+      <c r="E100" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B101" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="C101" s="6"/>
+      <c r="E101" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B102" s="6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="C102" s="6"/>
+      <c r="E102" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B103" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="C103" s="6"/>
+      <c r="E103" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B104" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="C104" s="6"/>
+      <c r="E104" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B105" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="C105" s="6"/>
+      <c r="E105" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B106" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="C106" s="6"/>
+      <c r="E106" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B107" s="6" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="C107" s="6"/>
+      <c r="E107" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B108" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C108" s="6" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="E108" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B109" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C109" s="6" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="E109" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B110" s="6" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="C110" s="6"/>
+      <c r="E110" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B111" s="6" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="C111" s="6"/>
+      <c r="E111" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B112" s="6" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="C112" s="6"/>
+      <c r="E112" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B113" s="6" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="C113" s="6"/>
+      <c r="E113" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B114" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="C114" s="6"/>
+      <c r="E114" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B115" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C115" s="6" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="E115" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B116" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="C116" s="9"/>
+      <c r="E116" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B117" s="9" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="C117" s="9"/>
+      <c r="E117" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B118" s="9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="C118" s="9"/>
+      <c r="E118" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B119" s="9" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="C119" s="9"/>
+      <c r="E119" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B120" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="C120" s="9"/>
+      <c r="E120" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B121" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="C121" s="9"/>
+      <c r="E121" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B122" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="C122" s="9"/>
+      <c r="E122" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B123" s="9" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="C123" s="9"/>
+      <c r="E123" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B124" s="9" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="C124" s="9"/>
+      <c r="E124" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B125" s="9" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="C125" s="9"/>
+      <c r="E125" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B126" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="C126" s="9"/>
+      <c r="E126" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B127" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="C127" s="9"/>
+      <c r="E127" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B128" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="C128" s="9"/>
+      <c r="E128" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B129" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="C129" s="9"/>
+      <c r="E129" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B130" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="C130" s="9"/>
+      <c r="E130" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B131" s="9" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="C131" s="9"/>
+      <c r="E131" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B132" s="9" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>123</v>
-      </c>
-      <c r="B96" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="C132" s="9"/>
+      <c r="E132" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B133" s="9" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+    </row>
+    <row r="134" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B134" s="9" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="C134" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D134" s="9"/>
+    </row>
+    <row r="135" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B135" s="9" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="C135" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D135" s="9"/>
+    </row>
+    <row r="136" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B136" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C136" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D136" s="9"/>
+    </row>
+    <row r="137" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C137" s="9" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>129</v>
-      </c>
-      <c r="B101" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="D137" s="9"/>
+    </row>
+    <row r="138" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B138" s="9" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+    </row>
+    <row r="139" spans="1:5" s="10" customFormat="1" ht="224" x14ac:dyDescent="0.2">
+      <c r="A139" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B139" s="9" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="C139" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D139" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B140" s="9" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+    </row>
+    <row r="141" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B141" s="9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+    </row>
+    <row r="142" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B142" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+    </row>
+    <row r="143" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B143" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+    </row>
+    <row r="144" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B144" s="9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+    </row>
+    <row r="145" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B145" s="9" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="C145" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D145" s="9"/>
+    </row>
+    <row r="146" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B146" s="9" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="C146" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D146" s="9"/>
+    </row>
+    <row r="147" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B147" s="9" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+    </row>
+    <row r="148" spans="1:4" s="10" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A148" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B148" s="9" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="C148" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D148" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B149" s="9" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+    </row>
+    <row r="150" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B150" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C150" s="9" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>143</v>
-      </c>
-      <c r="B115" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>145</v>
-      </c>
-      <c r="B116" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>146</v>
-      </c>
-      <c r="B117" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>147</v>
-      </c>
-      <c r="B118" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>148</v>
-      </c>
-      <c r="B119" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>149</v>
-      </c>
-      <c r="B120" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>151</v>
-      </c>
-      <c r="B121" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>153</v>
-      </c>
-      <c r="B122" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>155</v>
-      </c>
-      <c r="B123" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>156</v>
-      </c>
-      <c r="B124" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>157</v>
-      </c>
-      <c r="B125" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>158</v>
-      </c>
-      <c r="B126" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>159</v>
-      </c>
-      <c r="B127" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>160</v>
-      </c>
-      <c r="B128" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>161</v>
-      </c>
-      <c r="B129" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>163</v>
-      </c>
-      <c r="B130" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>165</v>
-      </c>
-      <c r="B131" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>167</v>
-      </c>
-      <c r="B132" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>168</v>
-      </c>
-      <c r="B133" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>170</v>
-      </c>
-      <c r="B134" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>171</v>
-      </c>
-      <c r="B135" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>172</v>
-      </c>
-      <c r="B136" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>173</v>
-      </c>
-      <c r="B137" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>174</v>
-      </c>
-      <c r="B138" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>175</v>
-      </c>
-      <c r="B139" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>176</v>
-      </c>
-      <c r="B140" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>177</v>
-      </c>
-      <c r="B141" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>178</v>
-      </c>
-      <c r="B142" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>179</v>
-      </c>
-      <c r="B143" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>181</v>
-      </c>
-      <c r="B144" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>183</v>
-      </c>
-      <c r="B145" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
-        <v>184</v>
-      </c>
-      <c r="B146" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>185</v>
-      </c>
-      <c r="B147" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>186</v>
-      </c>
-      <c r="B148" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>188</v>
-      </c>
-      <c r="B149" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>190</v>
-      </c>
-      <c r="B150" t="s">
-        <v>216</v>
-      </c>
+      <c r="D150" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009410E8-BE28-7D44-B242-F58C8D9F5002}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E5" t="s">
+        <v>258</v>
+      </c>
+      <c r="F5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E6" t="s">
+        <v>259</v>
+      </c>
+      <c r="F6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>309</v>
+      </c>
+      <c r="E7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" t="s">
+        <v>260</v>
+      </c>
+      <c r="F8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E9" t="s">
+        <v>270</v>
+      </c>
+      <c r="F9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" t="s">
+        <v>284</v>
+      </c>
+      <c r="E10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" t="s">
+        <v>285</v>
+      </c>
+      <c r="E11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" t="s">
+        <v>286</v>
+      </c>
+      <c r="E12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B13" t="s">
+        <v>287</v>
+      </c>
+      <c r="E13" t="s">
+        <v>272</v>
+      </c>
+      <c r="F13" t="s">
+        <v>277</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B14" t="s">
+        <v>288</v>
+      </c>
+      <c r="E14" t="s">
+        <v>273</v>
+      </c>
+      <c r="F14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>289</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>290</v>
+      </c>
+      <c r="E16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>291</v>
+      </c>
+      <c r="F17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>299</v>
+      </c>
+      <c r="F18" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>302</v>
+      </c>
+      <c r="F19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>303</v>
+      </c>
+      <c r="F20" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>304</v>
+      </c>
+      <c r="F21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>305</v>
+      </c>
+      <c r="F22" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>306</v>
+      </c>
+      <c r="F23" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:H6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Missing values html
</commit_message>
<xml_diff>
--- a/Codebook Uganda Panel.xlsx
+++ b/Codebook Uganda Panel.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/Master thesis/MLhetrogeneouseffects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78A343A-A46B-A542-B61E-B07D19CAE58E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDCEB2E-1BB8-024E-B1D7-00E54DA1D075}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="500" windowWidth="28040" windowHeight="16540" activeTab="1" xr2:uid="{4A1EAC35-01F1-A54B-8647-BEC3205DBE2C}"/>
+    <workbookView xWindow="2020" yWindow="500" windowWidth="28040" windowHeight="16540" activeTab="1" xr2:uid="{4A1EAC35-01F1-A54B-8647-BEC3205DBE2C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Code book" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>

</xml_diff>